<commit_message>
Actualizado WCAG.xlsx con version WCAG 2.2
</commit_message>
<xml_diff>
--- a/normas/English/WCAG.xlsx
+++ b/normas/English/WCAG.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34720C0E-0844-46B0-B5FF-7E7A78B946B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BF32CD-C4E4-4D46-8827-D68D8B7F36BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WCAG" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="249">
   <si>
     <t>WCAG</t>
   </si>
@@ -639,24 +639,7 @@
     </r>
   </si>
   <si>
-    <t>2.0</t>
-  </si>
-  <si>
     <t>A</t>
-  </si>
-  <si>
-    <r>
-      <t>4.1.1 Processing:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> In the content implemented through the use of brand languages, the elements have the full opening and closing tags; the elements are nested according to your specifications; elements do not contain duplicate attributes and IDs are unique, except when specifications allow these features.</t>
-    </r>
   </si>
   <si>
     <t>2.0</t>
@@ -2151,13 +2134,232 @@
   </si>
   <si>
     <t>This is an automatic translation from Spanish version of the archive available in GitHub</t>
+  </si>
+  <si>
+    <t>2.0 (Deleted in 2.2)</t>
+  </si>
+  <si>
+    <r>
+      <t>4.1.1 Processing:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>In the content implemented through the use of brand languages, the elements have the full opening and closing tags; the elements are nested according to your specifications; elements do not contain duplicate attributes and IDs are unique, except when specifications allow these features.</t>
+    </r>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2.4.11 Focus Not Obscured (Minimum)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: When a user interface component receives keyboard focus, the component is not entirely hidden due to author-created content.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2.4.12 Focus Not Obscured (Enhanced)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: When a user interface component receives keyboard focus, no part of the component is hidden by author-created content.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2.4.13 Focus Appearance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: When the keyboard focus indicator is visible, an area of the focus indicator meets all the following: is at least as large as the area of a 2 CSS pixel thick perimeter of the unfocused component or sub-component, and has a contrast ratio of at least 3:1 between the same pixels in the focused and unfocused states. Exceptions: The focus indicator is determined by the user agent and cannot be adjusted by the author, or The focus indicator and the indicator's background color are not modified by the author.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2.5.7 Dragging Movements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: All functionality that uses a dragging movement for operation can be achieved by a single pointer without dragging, unless dragging is essential or the functionality is determined by the user agent and not modified by the author.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2.5.8 Target Size (Minimum)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: The size of the target for pointer inputs is at least 24 by 24 CSS pixels, except where: Spacing: Undersized targets (those less than 24 by 24 CSS pixels) are positioned so that if a 24 CSS pixel diameter circle is centered on the bounding box of each, the circles do not intersect another target or the circle for another undersized target; Equivalent: The function can be achieved through a different control on the same page that meets this criterion; Inline: The target is in a sentence or its size is otherwise constrained by the line-height of non-target text; User agent control: The size of the target is determined by the user agent and is not modified by the author; Essential: A particular presentation of the target is essential or is legally required for the information being conveyed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3.2.6 Consistent Help</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: If a Web page contains any of the following help mechanisms, and those mechanisms are repeated on multiple Web pages within a set of Web pages, they occur in the same order relative to other page content, unless a change is initiated by the user: Human contact details; Human contact mechanism; Self-help option; A fully automated contact mechanism.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3.3.7 Redundant Entry</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Information previously entered by or provided to the user that is required to be entered again in the same process is either: auto-populated, or available for the user to select. Except when: re-entering the information is essential, the information is required to ensure the security of the content, or previously entered information is no longer valid.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3.3.8 Accessible Authentication (Minimum)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: A cognitive function test (such as remembering a password or solving a puzzle) is not required for any step in an authentication process unless that step provides at least one of the following: Alternative: Another authentication method that does not rely on a cognitive function test; Mechanism: A mechanism is available to assist the user in completing the cognitive function test; Object Recognition; The cognitive function test is to recognize objects; Personal Content: The cognitive function test is to identify non-text content the user provided to the Web site.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3.3.9 Accessible Authentication (Enhanced)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: A cognitive function test (such as remembering a password or solving a puzzle) is not required for any step in an authentication process unless that step provides at least one of the following: Alternative: Another authentication method that does not rely on a cognitive function test; Mechanism: A mechanism is available to assist the user in completing the cognitive function test.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2213,6 +2415,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2256,7 +2465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2278,9 +2487,6 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2314,6 +2520,12 @@
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2361,9 +2573,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2401,9 +2613,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2436,26 +2648,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2488,26 +2683,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2681,36 +2859,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="6"/>
+    <col min="1" max="1" width="10.5546875" style="6" customWidth="1"/>
     <col min="2" max="2" width="9.44140625" style="6" customWidth="1"/>
     <col min="3" max="3" width="161.88671875" style="6" customWidth="1"/>
     <col min="4" max="16384" width="9.109375" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>236</v>
+      <c r="C1" s="11" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2718,10 +2896,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="45.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2729,10 +2907,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -2740,834 +2918,933 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="13" spans="1:3" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="14" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+    <row r="15" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="61.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+    <row r="19" spans="1:3" ht="45.6" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="60.6" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="75.599999999999994" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="60.6" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="75.599999999999994" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B31" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45.6" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+    <row r="32" spans="1:3" ht="45.6" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B32" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+    <row r="33" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="60.6" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="90.6" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B35" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="75.599999999999994" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+    <row r="36" spans="1:3" ht="75.599999999999994" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B36" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+    <row r="37" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B41" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B44" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+    <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="60.6" x14ac:dyDescent="0.25">
+      <c r="A48" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B49" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+    <row r="50" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B50" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+    <row r="51" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B51" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+    <row r="52" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="60.6" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="60.6" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A63" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="90.6" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A65" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B65" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+    <row r="66" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A66" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A69" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A70" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B71" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+    <row r="72" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A72" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B72" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
+    <row r="73" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="45.6" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B77" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+    <row r="78" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B78" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C78" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+    <row r="79" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="60.6" x14ac:dyDescent="0.25">
+      <c r="A80" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="45.6" x14ac:dyDescent="0.25">
+      <c r="A82" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="45.6" x14ac:dyDescent="0.25">
+      <c r="A83" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="60.6" x14ac:dyDescent="0.25">
+      <c r="A84" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="45.6" x14ac:dyDescent="0.25">
+      <c r="A85" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="B86" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="C86" s="21" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="45.6" x14ac:dyDescent="0.25">
+      <c r="A87" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="B87" s="10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="45.6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="C87" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="60.6" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="60.6" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="45.6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="60.6" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="61.8" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="C46" s="16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="45.6" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C47" s="17" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="60.6" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="75.599999999999994" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="C49" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="105.6" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="B50" s="14" t="s">
+    </row>
+    <row r="88" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
+      <c r="A88" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="B88" s="13" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+      <c r="C88" s="18" t="s">
         <v>149</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="B53" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B54" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="B55" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="B56" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="60.6" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="75.599999999999994" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="B58" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="B60" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="B63" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="B65" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="C65" s="11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="B67" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="B71" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>213</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="B73" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="45.6" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="B74" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="C74" s="13" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="B76" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="C76" s="11" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="B77" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="C77" s="11" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="60.6" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="B79" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="C79" s="11" t="s">
-        <v>235</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C62" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C79">
-      <sortCondition ref="B1:B62"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C88">
+      <sortCondition ref="C1:C62"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3579,20 +3856,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCC91DD-E427-4BC5-AEF7-0C77B9110736}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>237</v>
+      <c r="A1" s="19" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
-        <v>238</v>
+      <c r="A2" s="19" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>